<commit_message>
query and target variables
</commit_message>
<xml_diff>
--- a/example_output_PSL.xlsx
+++ b/example_output_PSL.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t># tStarts - Comma-separated list of start position of each block in target.</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">mis- </t>
+  </si>
+  <si>
+    <t>sum of blockSizes = match+mis-match</t>
   </si>
 </sst>
 </file>
@@ -620,7 +623,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1355,17 +1358,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>

</xml_diff>